<commit_message>
functionality completed by modifying the code in app.js and cdms.js
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\backend\Classroom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B812A20-3B5B-4FBF-B44B-2199380A85EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91148B1-2DC1-421C-8EF7-2976918C7CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>CY</t>
+  </si>
+  <si>
+    <t>student6</t>
+  </si>
+  <si>
+    <t>CD</t>
   </si>
 </sst>
 </file>
@@ -375,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,6 +473,20 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>